<commit_message>
fix formatting on spreadsheet
</commit_message>
<xml_diff>
--- a/guidance/assessment/2017-ws-self-assessment-results.xlsx
+++ b/guidance/assessment/2017-ws-self-assessment-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15960"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manual tests" sheetId="1" r:id="rId1"/>
@@ -268,19 +268,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF5C6E81"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -315,6 +302,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF5C6E81"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -724,9 +723,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -734,7 +733,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -760,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -781,8 +780,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -798,34 +797,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -856,7 +845,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -888,28 +877,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -917,6 +906,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1222,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="M34" workbookViewId="0">
+      <selection activeCell="W71" sqref="W71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1261,91 +1259,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="71" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="73" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="74"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
     </row>
     <row r="2" spans="1:30" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="75" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="69" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69" t="s">
+      <c r="T2" s="66"/>
+      <c r="U2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="70"/>
-      <c r="W2" s="69" t="s">
+      <c r="V2" s="66"/>
+      <c r="W2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="69" t="s">
+      <c r="X2" s="66"/>
+      <c r="Y2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="70"/>
+      <c r="Z2" s="66"/>
     </row>
     <row r="3" spans="1:30" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="50" t="s">
+      <c r="C3" s="72"/>
+      <c r="D3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="43" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1387,39 +1385,39 @@
       <c r="R3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="62" t="s">
+      <c r="S3" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="63" t="s">
+      <c r="T3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="62" t="s">
+      <c r="U3" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="63" t="s">
+      <c r="V3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="W3" s="62" t="s">
+      <c r="W3" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="63" t="s">
+      <c r="X3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="Y3" s="62" t="s">
+      <c r="Y3" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="63" t="s">
+      <c r="Z3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="44"/>
+      <c r="AA3" s="40"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="41">
+      <c r="A4" s="37">
         <v>1</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="32" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="20" t="s">
@@ -1451,10 +1449,10 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="32" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="20" t="s">
@@ -1482,51 +1480,51 @@
       <c r="V5" s="9"/>
       <c r="W5" s="8"/>
       <c r="X5" s="9"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="55"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="51"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="34" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="37"/>
+      <c r="E6" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="33"/>
       <c r="R6" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="57"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="52"/>
+      <c r="Z6" s="53"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="41">
+      <c r="A7" s="37">
         <v>2</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="32" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="20" t="s">
@@ -1558,10 +1556,10 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="32" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="20" t="s">
@@ -1589,51 +1587,51 @@
       <c r="V8" s="9"/>
       <c r="W8" s="8"/>
       <c r="X8" s="9"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="55"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="51"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="34" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
+      <c r="E9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="33"/>
       <c r="R9" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S9" s="36"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="56"/>
-      <c r="Z9" s="57"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="53"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="41">
+      <c r="A10" s="37">
         <v>3</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="32" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="20" t="s">
@@ -1665,10 +1663,10 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="32" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="20" t="s">
@@ -1696,51 +1694,51 @@
       <c r="V11" s="9"/>
       <c r="W11" s="8"/>
       <c r="X11" s="9"/>
-      <c r="Y11" s="54"/>
-      <c r="Z11" s="55"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="51"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="34" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="37"/>
+      <c r="E12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="33"/>
       <c r="R12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S12" s="36"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="37"/>
-      <c r="Y12" s="56"/>
-      <c r="Z12" s="57"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="53"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="41">
+      <c r="A13" s="37">
         <v>4</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="32" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="20" t="s">
@@ -1772,10 +1770,10 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="32" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="20" t="s">
@@ -1803,51 +1801,51 @@
       <c r="V14" s="9"/>
       <c r="W14" s="8"/>
       <c r="X14" s="9"/>
-      <c r="Y14" s="54"/>
-      <c r="Z14" s="55"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="51"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="43"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="34" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="37"/>
+      <c r="E15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="33"/>
       <c r="R15" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S15" s="36"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="56"/>
-      <c r="Z15" s="57"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="53"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="41">
+      <c r="A16" s="37">
         <v>5</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="32" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="20" t="s">
@@ -1879,10 +1877,10 @@
       <c r="Z16" s="9"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="32" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="20" t="s">
@@ -1910,51 +1908,51 @@
       <c r="V17" s="9"/>
       <c r="W17" s="8"/>
       <c r="X17" s="9"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="55"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="51"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="43"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="34" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="37"/>
+      <c r="E18" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="33"/>
       <c r="R18" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S18" s="36"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="56"/>
-      <c r="Z18" s="57"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="52"/>
+      <c r="Z18" s="53"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="41">
+      <c r="A19" s="37">
         <v>6</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="32" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="20" t="s">
@@ -1986,10 +1984,10 @@
       <c r="Z19" s="9"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="32" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="20" t="s">
@@ -2017,51 +2015,51 @@
       <c r="V20" s="9"/>
       <c r="W20" s="8"/>
       <c r="X20" s="9"/>
-      <c r="Y20" s="54"/>
-      <c r="Z20" s="55"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="51"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="43"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="34" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="37"/>
+      <c r="E21" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="33"/>
       <c r="R21" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S21" s="36"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="57"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="33"/>
+      <c r="Y21" s="52"/>
+      <c r="Z21" s="53"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="41">
+      <c r="A22" s="37">
         <v>7</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="32" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="20" t="s">
@@ -2093,10 +2091,10 @@
       <c r="Z22" s="9"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="32" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -2124,51 +2122,51 @@
       <c r="V23" s="9"/>
       <c r="W23" s="8"/>
       <c r="X23" s="9"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="55"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="51"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="43"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="34" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="37"/>
+      <c r="E24" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="33"/>
       <c r="R24" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S24" s="36"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="57"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="53"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="41">
+      <c r="A25" s="37">
         <v>8</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="32" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="20" t="s">
@@ -2200,10 +2198,10 @@
       <c r="Z25" s="9"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="32" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="20" t="s">
@@ -2231,51 +2229,51 @@
       <c r="V26" s="9"/>
       <c r="W26" s="8"/>
       <c r="X26" s="9"/>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="55"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="51"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="43"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="34" t="s">
+      <c r="A27" s="39"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="37"/>
+      <c r="E27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="33"/>
       <c r="R27" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S27" s="36"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="57"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="53"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="41">
+      <c r="A28" s="37">
         <v>9</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="32" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="20" t="s">
@@ -2307,10 +2305,10 @@
       <c r="Z28" s="9"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="32" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="20" t="s">
@@ -2338,51 +2336,51 @@
       <c r="V29" s="9"/>
       <c r="W29" s="8"/>
       <c r="X29" s="9"/>
-      <c r="Y29" s="54"/>
-      <c r="Z29" s="55"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="51"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="34" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="37"/>
+      <c r="E30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="33"/>
       <c r="R30" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S30" s="36"/>
-      <c r="T30" s="37"/>
-      <c r="U30" s="36"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="37"/>
-      <c r="Y30" s="56"/>
-      <c r="Z30" s="57"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="53"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="41">
+      <c r="A31" s="37">
         <v>10</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="32" t="s">
+      <c r="B31" s="29"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="20" t="s">
@@ -2414,10 +2412,10 @@
       <c r="Z31" s="9"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="32" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -2445,51 +2443,51 @@
       <c r="V32" s="9"/>
       <c r="W32" s="8"/>
       <c r="X32" s="9"/>
-      <c r="Y32" s="54"/>
-      <c r="Z32" s="55"/>
+      <c r="Y32" s="50"/>
+      <c r="Z32" s="51"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="43"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="34" t="s">
+      <c r="A33" s="39"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="37"/>
+      <c r="E33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="33"/>
       <c r="R33" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S33" s="36"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="36"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="57"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="33"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="33"/>
+      <c r="Y33" s="52"/>
+      <c r="Z33" s="53"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="41">
+      <c r="A34" s="37">
         <v>11</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="32" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="20" t="s">
@@ -2521,10 +2519,10 @@
       <c r="Z34" s="9"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="32" t="s">
+      <c r="A35" s="38"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="20" t="s">
@@ -2552,51 +2550,51 @@
       <c r="V35" s="9"/>
       <c r="W35" s="8"/>
       <c r="X35" s="9"/>
-      <c r="Y35" s="54"/>
-      <c r="Z35" s="55"/>
+      <c r="Y35" s="50"/>
+      <c r="Z35" s="51"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="43"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="34" t="s">
+      <c r="A36" s="39"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="37"/>
+      <c r="E36" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="33"/>
       <c r="R36" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S36" s="36"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="36"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="56"/>
-      <c r="Z36" s="57"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="33"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="33"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="33"/>
+      <c r="Y36" s="52"/>
+      <c r="Z36" s="53"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="41">
+      <c r="A37" s="37">
         <v>12</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="32" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="20" t="s">
@@ -2628,10 +2626,10 @@
       <c r="Z37" s="9"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="32" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="20" t="s">
@@ -2659,51 +2657,51 @@
       <c r="V38" s="9"/>
       <c r="W38" s="8"/>
       <c r="X38" s="9"/>
-      <c r="Y38" s="54"/>
-      <c r="Z38" s="55"/>
+      <c r="Y38" s="50"/>
+      <c r="Z38" s="51"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="43"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="34" t="s">
+      <c r="A39" s="39"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F39" s="36"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="37"/>
+      <c r="E39" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="33"/>
       <c r="R39" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S39" s="36"/>
-      <c r="T39" s="37"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="37"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="37"/>
-      <c r="Y39" s="56"/>
-      <c r="Z39" s="57"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="33"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="33"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="33"/>
+      <c r="Y39" s="52"/>
+      <c r="Z39" s="53"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="41">
+      <c r="A40" s="37">
         <v>13</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="32" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="20" t="s">
@@ -2735,10 +2733,10 @@
       <c r="Z40" s="9"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="32" t="s">
+      <c r="A41" s="38"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="20" t="s">
@@ -2766,51 +2764,51 @@
       <c r="V41" s="9"/>
       <c r="W41" s="8"/>
       <c r="X41" s="9"/>
-      <c r="Y41" s="54"/>
-      <c r="Z41" s="55"/>
+      <c r="Y41" s="50"/>
+      <c r="Z41" s="51"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="43"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="34" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" s="36"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="37"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="37"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="37"/>
+      <c r="E42" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="33"/>
       <c r="R42" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S42" s="36"/>
-      <c r="T42" s="37"/>
-      <c r="U42" s="36"/>
-      <c r="V42" s="37"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="37"/>
-      <c r="Y42" s="56"/>
-      <c r="Z42" s="57"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="33"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="33"/>
+      <c r="W42" s="32"/>
+      <c r="X42" s="33"/>
+      <c r="Y42" s="52"/>
+      <c r="Z42" s="53"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="41">
+      <c r="A43" s="37">
         <v>14</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="32" t="s">
+      <c r="B43" s="29"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="20" t="s">
@@ -2842,10 +2840,10 @@
       <c r="Z43" s="9"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="42"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="32" t="s">
+      <c r="A44" s="38"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E44" s="20" t="s">
@@ -2873,51 +2871,51 @@
       <c r="V44" s="9"/>
       <c r="W44" s="8"/>
       <c r="X44" s="9"/>
-      <c r="Y44" s="54"/>
-      <c r="Z44" s="55"/>
+      <c r="Y44" s="50"/>
+      <c r="Z44" s="51"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="43"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="34" t="s">
+      <c r="A45" s="39"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="36"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="36"/>
-      <c r="O45" s="37"/>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="37"/>
+      <c r="E45" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="32"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="33"/>
       <c r="R45" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S45" s="36"/>
-      <c r="T45" s="37"/>
-      <c r="U45" s="36"/>
-      <c r="V45" s="37"/>
-      <c r="W45" s="36"/>
-      <c r="X45" s="37"/>
-      <c r="Y45" s="56"/>
-      <c r="Z45" s="57"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="33"/>
+      <c r="U45" s="32"/>
+      <c r="V45" s="33"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="33"/>
+      <c r="Y45" s="52"/>
+      <c r="Z45" s="53"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="41">
+      <c r="A46" s="37">
         <v>15</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="32" t="s">
+      <c r="B46" s="29"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="20" t="s">
@@ -2949,10 +2947,10 @@
       <c r="Z46" s="9"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="42"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="32" t="s">
+      <c r="A47" s="38"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E47" s="20" t="s">
@@ -2980,51 +2978,51 @@
       <c r="V47" s="9"/>
       <c r="W47" s="8"/>
       <c r="X47" s="9"/>
-      <c r="Y47" s="54"/>
-      <c r="Z47" s="55"/>
+      <c r="Y47" s="50"/>
+      <c r="Z47" s="51"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="34" t="s">
+      <c r="A48" s="39"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F48" s="36"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="37"/>
+      <c r="E48" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="32"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="33"/>
       <c r="R48" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S48" s="36"/>
-      <c r="T48" s="37"/>
-      <c r="U48" s="36"/>
-      <c r="V48" s="37"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="37"/>
-      <c r="Y48" s="56"/>
-      <c r="Z48" s="57"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="33"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="33"/>
+      <c r="W48" s="32"/>
+      <c r="X48" s="33"/>
+      <c r="Y48" s="52"/>
+      <c r="Z48" s="53"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="41">
+      <c r="A49" s="37">
         <v>16</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="32" t="s">
+      <c r="B49" s="29"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="20" t="s">
@@ -3056,10 +3054,10 @@
       <c r="Z49" s="9"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="32" t="s">
+      <c r="A50" s="38"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="20" t="s">
@@ -3087,51 +3085,51 @@
       <c r="V50" s="9"/>
       <c r="W50" s="8"/>
       <c r="X50" s="9"/>
-      <c r="Y50" s="54"/>
-      <c r="Z50" s="55"/>
+      <c r="Y50" s="50"/>
+      <c r="Z50" s="51"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="34" t="s">
+      <c r="A51" s="39"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E51" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" s="36"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="37"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="37"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="37"/>
+      <c r="E51" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="32"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="32"/>
+      <c r="Q51" s="33"/>
       <c r="R51" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S51" s="36"/>
-      <c r="T51" s="37"/>
-      <c r="U51" s="36"/>
-      <c r="V51" s="37"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="37"/>
-      <c r="Y51" s="56"/>
-      <c r="Z51" s="57"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="33"/>
+      <c r="U51" s="32"/>
+      <c r="V51" s="33"/>
+      <c r="W51" s="32"/>
+      <c r="X51" s="33"/>
+      <c r="Y51" s="52"/>
+      <c r="Z51" s="53"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="41">
+      <c r="A52" s="37">
         <v>17</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="32" t="s">
+      <c r="B52" s="29"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E52" s="20" t="s">
@@ -3163,10 +3161,10 @@
       <c r="Z52" s="9"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="32" t="s">
+      <c r="A53" s="38"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E53" s="20" t="s">
@@ -3194,51 +3192,51 @@
       <c r="V53" s="9"/>
       <c r="W53" s="8"/>
       <c r="X53" s="9"/>
-      <c r="Y53" s="54"/>
-      <c r="Z53" s="55"/>
+      <c r="Y53" s="50"/>
+      <c r="Z53" s="51"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="43"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="34" t="s">
+      <c r="A54" s="39"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F54" s="36"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="36"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="36"/>
-      <c r="O54" s="37"/>
-      <c r="P54" s="36"/>
-      <c r="Q54" s="37"/>
+      <c r="E54" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="32"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="32"/>
+      <c r="Q54" s="33"/>
       <c r="R54" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S54" s="36"/>
-      <c r="T54" s="37"/>
-      <c r="U54" s="36"/>
-      <c r="V54" s="37"/>
-      <c r="W54" s="36"/>
-      <c r="X54" s="37"/>
-      <c r="Y54" s="56"/>
-      <c r="Z54" s="57"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="33"/>
+      <c r="U54" s="32"/>
+      <c r="V54" s="33"/>
+      <c r="W54" s="32"/>
+      <c r="X54" s="33"/>
+      <c r="Y54" s="52"/>
+      <c r="Z54" s="53"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55" s="41">
+      <c r="A55" s="37">
         <v>18</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="67"/>
-      <c r="D55" s="32" t="s">
+      <c r="B55" s="29"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E55" s="20" t="s">
@@ -3270,10 +3268,10 @@
       <c r="Z55" s="9"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A56" s="42"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="32" t="s">
+      <c r="A56" s="38"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="20" t="s">
@@ -3301,51 +3299,51 @@
       <c r="V56" s="9"/>
       <c r="W56" s="8"/>
       <c r="X56" s="9"/>
-      <c r="Y56" s="54"/>
-      <c r="Z56" s="55"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="51"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A57" s="43"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="34" t="s">
+      <c r="A57" s="39"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" s="36"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="37"/>
-      <c r="N57" s="36"/>
-      <c r="O57" s="37"/>
-      <c r="P57" s="36"/>
-      <c r="Q57" s="37"/>
+      <c r="E57" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="32"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="33"/>
+      <c r="N57" s="32"/>
+      <c r="O57" s="33"/>
+      <c r="P57" s="32"/>
+      <c r="Q57" s="33"/>
       <c r="R57" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S57" s="36"/>
-      <c r="T57" s="37"/>
-      <c r="U57" s="36"/>
-      <c r="V57" s="37"/>
-      <c r="W57" s="36"/>
-      <c r="X57" s="37"/>
-      <c r="Y57" s="56"/>
-      <c r="Z57" s="57"/>
+      <c r="S57" s="32"/>
+      <c r="T57" s="33"/>
+      <c r="U57" s="32"/>
+      <c r="V57" s="33"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="33"/>
+      <c r="Y57" s="52"/>
+      <c r="Z57" s="53"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58" s="41">
+      <c r="A58" s="37">
         <v>19</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="67"/>
-      <c r="D58" s="32" t="s">
+      <c r="B58" s="29"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="20" t="s">
@@ -3377,10 +3375,10 @@
       <c r="Z58" s="9"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A59" s="42"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="32" t="s">
+      <c r="A59" s="38"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E59" s="20" t="s">
@@ -3408,51 +3406,51 @@
       <c r="V59" s="9"/>
       <c r="W59" s="8"/>
       <c r="X59" s="9"/>
-      <c r="Y59" s="54"/>
-      <c r="Z59" s="55"/>
+      <c r="Y59" s="50"/>
+      <c r="Z59" s="51"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A60" s="43"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="34" t="s">
+      <c r="A60" s="39"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" s="36"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="36"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="36"/>
-      <c r="O60" s="37"/>
-      <c r="P60" s="36"/>
-      <c r="Q60" s="37"/>
+      <c r="E60" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="32"/>
+      <c r="Q60" s="33"/>
       <c r="R60" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S60" s="36"/>
-      <c r="T60" s="37"/>
-      <c r="U60" s="36"/>
-      <c r="V60" s="37"/>
-      <c r="W60" s="36"/>
-      <c r="X60" s="37"/>
-      <c r="Y60" s="56"/>
-      <c r="Z60" s="57"/>
+      <c r="S60" s="32"/>
+      <c r="T60" s="33"/>
+      <c r="U60" s="32"/>
+      <c r="V60" s="33"/>
+      <c r="W60" s="32"/>
+      <c r="X60" s="33"/>
+      <c r="Y60" s="52"/>
+      <c r="Z60" s="53"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A61" s="41">
+      <c r="A61" s="37">
         <v>20</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="67"/>
-      <c r="D61" s="32" t="s">
+      <c r="B61" s="29"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E61" s="20" t="s">
@@ -3484,10 +3482,10 @@
       <c r="Z61" s="9"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A62" s="42"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="32" t="s">
+      <c r="A62" s="38"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E62" s="20" t="s">
@@ -3515,14 +3513,14 @@
       <c r="V62" s="9"/>
       <c r="W62" s="8"/>
       <c r="X62" s="9"/>
-      <c r="Y62" s="54"/>
-      <c r="Z62" s="55"/>
+      <c r="Y62" s="50"/>
+      <c r="Z62" s="51"/>
     </row>
     <row r="63" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="31" t="s">
+      <c r="A63" s="39"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="27" t="s">
         <v>21</v>
       </c>
       <c r="E63" s="21" t="s">
@@ -3550,8 +3548,8 @@
       <c r="V63" s="11"/>
       <c r="W63" s="10"/>
       <c r="X63" s="11"/>
-      <c r="Y63" s="58"/>
-      <c r="Z63" s="59"/>
+      <c r="Y63" s="54"/>
+      <c r="Z63" s="55"/>
     </row>
     <row r="64" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="5:26" x14ac:dyDescent="0.2">
@@ -3757,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3856,76 +3854,76 @@
       <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>

</xml_diff>

<commit_message>
fix formula in spreadsheet
</commit_message>
<xml_diff>
--- a/guidance/assessment/2017-ws-self-assessment-results.xlsx
+++ b/guidance/assessment/2017-ws-self-assessment-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="Manual tests" sheetId="1" r:id="rId1"/>
@@ -223,12 +223,6 @@
     <t>2. Contact</t>
   </si>
   <si>
-    <t>Only run this test if the page is a  home page</t>
-  </si>
-  <si>
-    <t>Only run this test if the page is a contact page</t>
-  </si>
-  <si>
     <t>Run this test on all pages</t>
   </si>
   <si>
@@ -239,6 +233,12 @@
   </si>
   <si>
     <t>4. Printable</t>
+  </si>
+  <si>
+    <t>Only run this test on a home page</t>
+  </si>
+  <si>
+    <t>Only run this test on a contact page</t>
   </si>
 </sst>
 </file>
@@ -883,6 +883,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -900,21 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1220,14 +1220,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView topLeftCell="M34" workbookViewId="0">
-      <selection activeCell="W71" sqref="W71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="36.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="33.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
@@ -1263,11 +1264,11 @@
       <c r="B1" s="47"/>
       <c r="C1" s="60"/>
       <c r="D1" s="45"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
       <c r="H1" s="41"/>
       <c r="I1" s="41"/>
       <c r="J1" s="41"/>
@@ -1279,10 +1280,10 @@
       <c r="P1" s="41"/>
       <c r="Q1" s="41"/>
       <c r="R1" s="41"/>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="70"/>
+      <c r="T1" s="75"/>
       <c r="U1" s="57"/>
       <c r="V1" s="57"/>
       <c r="W1" s="57"/>
@@ -1297,8 +1298,8 @@
     <row r="2" spans="1:30" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42"/>
       <c r="B2" s="47"/>
-      <c r="C2" s="71" t="s">
-        <v>32</v>
+      <c r="C2" s="68" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="45"/>
       <c r="E2" s="49"/>
@@ -1315,22 +1316,22 @@
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
       <c r="R2" s="41"/>
-      <c r="S2" s="65" t="s">
+      <c r="S2" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="71"/>
+      <c r="U2" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="71"/>
+      <c r="W2" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="66"/>
-      <c r="U2" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="66"/>
-      <c r="W2" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="66"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="71"/>
     </row>
     <row r="3" spans="1:30" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
@@ -1339,7 +1340,7 @@
       <c r="B3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="72"/>
+      <c r="C3" s="69"/>
       <c r="D3" s="46" t="s">
         <v>18</v>
       </c>
@@ -1398,13 +1399,13 @@
         <v>4</v>
       </c>
       <c r="W3" s="58" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X3" s="59" t="s">
         <v>4</v>
       </c>
       <c r="Y3" s="58" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z3" s="59" t="s">
         <v>4</v>
@@ -3562,22 +3563,27 @@
       </c>
       <c r="G65" s="23"/>
       <c r="H65" s="22">
+        <f>COUNTIF(H$4:H$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="I65" s="23"/>
       <c r="J65" s="22">
+        <f>COUNTIF(J$4:J$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="K65" s="23"/>
       <c r="L65" s="22">
+        <f>COUNTIF(L$4:L$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="M65" s="23"/>
       <c r="N65" s="22">
+        <f>COUNTIF(N$4:N$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="O65" s="23"/>
       <c r="P65" s="22">
+        <f>COUNTIF(P$4:P$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="Q65" s="19"/>
@@ -3587,14 +3593,17 @@
       </c>
       <c r="T65" s="23"/>
       <c r="U65" s="22">
+        <f>COUNTIF(U$4:U$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="V65" s="23"/>
       <c r="W65" s="22">
+        <f>COUNTIF(W$4:W$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="X65" s="23"/>
       <c r="Y65" s="22">
+        <f>COUNTIF(Y$4:Y$63,"Pass")</f>
         <v>0</v>
       </c>
       <c r="Z65" s="19"/>
@@ -3609,22 +3618,27 @@
       </c>
       <c r="G66" s="25"/>
       <c r="H66" s="24">
+        <f>COUNTIF(H$4:H$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="I66" s="25"/>
       <c r="J66" s="24">
+        <f>COUNTIF(J$4:J$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="K66" s="25"/>
       <c r="L66" s="24">
+        <f>COUNTIF(L$4:L$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="M66" s="25"/>
       <c r="N66" s="24">
+        <f>COUNTIF(N$4:N$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="O66" s="25"/>
       <c r="P66" s="24">
+        <f>COUNTIF(P$4:P$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="Q66" s="17"/>
@@ -3634,14 +3648,17 @@
       </c>
       <c r="T66" s="25"/>
       <c r="U66" s="24">
+        <f>COUNTIF(U$4:U$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="V66" s="25"/>
       <c r="W66" s="24">
+        <f>COUNTIF(W$4:W$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="X66" s="25"/>
       <c r="Y66" s="24">
+        <f>COUNTIF(Y$4:Y$63,"Fail")</f>
         <v>0</v>
       </c>
       <c r="Z66" s="17"/>
@@ -3755,7 +3772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3854,76 +3871,76 @@
       <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>

</xml_diff>